<commit_message>
partition functionの計算をmillar et al. 2010の式(5)と統一
</commit_message>
<xml_diff>
--- a/赤外カメラ観測見積もり.xlsx
+++ b/赤外カメラ観測見積もり.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f068043b4f6ccc76/Documents/PPARC/IR_camera_ESPRIT/観測見積もり/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1776" documentId="8_{EB37A21E-167B-460E-AD36-770B7C3064F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D95E2C9-D83B-4414-99DA-1A26618147F3}"/>
+  <xr:revisionPtr revIDLastSave="1806" documentId="8_{EB37A21E-167B-460E-AD36-770B7C3064F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{64AC066A-48CD-47BC-B662-EB5EAF27DAAC}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{9CDB5083-10E1-4F1D-BEF8-63AEB4958B60}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9CDB5083-10E1-4F1D-BEF8-63AEB4958B60}"/>
   </bookViews>
   <sheets>
     <sheet name="SN計算（新）" sheetId="3" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="200">
   <si>
     <t>システムゲイン</t>
     <phoneticPr fontId="1"/>
@@ -1194,6 +1194,13 @@
   </si>
   <si>
     <t>A_6</t>
+  </si>
+  <si>
+    <t>Partition functionの係数</t>
+    <rPh sb="19" eb="21">
+      <t>ケイスウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -1980,8 +1987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E064F073-BF80-4605-AA24-B9D133186576}">
   <dimension ref="B1:X49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T26" sqref="T26"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -2001,6 +2008,7 @@
     <col min="18" max="18" width="11.75" style="36" customWidth="1"/>
     <col min="19" max="19" width="10.875" customWidth="1"/>
     <col min="20" max="20" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.25" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="11.125" style="38" customWidth="1"/>
     <col min="23" max="23" width="10.5" style="39" customWidth="1"/>
     <col min="24" max="24" width="13.375" bestFit="1" customWidth="1"/>
@@ -2204,27 +2212,27 @@
       <c r="I5" s="43">
         <v>2552.5691000000002</v>
       </c>
-      <c r="K5" s="32" t="e">
+      <c r="K5" s="32">
         <f t="shared" ref="K5:K16" si="0">$F$27 * F5 * (2*G5+1) *$X$20*$X$19*(E5*10^2)*H5 * EXP(-((I5*10^2) * $X$20*$X$19)/($X$21*$F$20)) / (4*PI()*$X$23)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L5" s="44" t="e">
+        <v>6.3749588734207388E-7</v>
+      </c>
+      <c r="L5" s="44">
         <f t="shared" ref="L5:L16" si="1">((K5 * $R$20 * $L$19 * $R$32 * $R$33) / ($X$20 * $X$19/(D5*10^-6))) * $L$20 * (1/$L$25) * $F$26 * $L$31</f>
-        <v>#DIV/0!</v>
+        <v>6592.1846117059022</v>
       </c>
       <c r="M5" s="44">
         <f t="shared" ref="M5:M16" si="2">(($F$28 * $R$20 * $L$19 * $R$33) / ($X$20 * $X$19/(D5*10^-6))) * $L$20 * (1/$L$25) * $F$26 * $L$31</f>
         <v>34354.26430955001</v>
       </c>
-      <c r="N5" s="45" t="e">
+      <c r="N5" s="45">
         <f>L5/SQRT(L5 + M5 + $L$26 + ($F$23/$L$25)^2*$L$31)</f>
-        <v>#DIV/0!</v>
+        <v>29.826343904301439</v>
       </c>
       <c r="O5" s="44"/>
       <c r="R5" s="46"/>
-      <c r="S5" s="43" t="e">
+      <c r="S5" s="43">
         <f>L5/N5</f>
-        <v>#DIV/0!</v>
+        <v>221.01886281661237</v>
       </c>
       <c r="V5" s="47"/>
       <c r="W5" s="48"/>
@@ -2253,54 +2261,54 @@
       <c r="I6" s="43">
         <v>2961.84</v>
       </c>
-      <c r="K6" s="32" t="e">
+      <c r="K6" s="32">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L6" s="44" t="e">
+        <v>1.4366877363882608E-6</v>
+      </c>
+      <c r="L6" s="44">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>14978.570142634622</v>
       </c>
       <c r="M6" s="44">
         <f t="shared" si="2"/>
         <v>34636.71146109578</v>
       </c>
-      <c r="N6" s="45" t="e">
+      <c r="N6" s="45">
         <f t="shared" ref="N6:N16" si="4">L6/SQRT(L6 + M6 + $L$26*$L$31 + ($F$23/$L$25)^2*$L$31)</f>
-        <v>#DIV/0!</v>
+        <v>57.52761201081227</v>
       </c>
       <c r="O6" s="44"/>
       <c r="P6">
         <f>(F6*(2*G6+1)*E6*H6) / (F$5*(2*G$5+1)*E$5*H$5)</f>
         <v>6.0132395889515431</v>
       </c>
-      <c r="Q6" s="24" t="e">
+      <c r="Q6" s="24">
         <f>L6/$L$5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R6" s="36" t="e">
+        <v>2.2721709152436071</v>
+      </c>
+      <c r="R6" s="36">
         <f t="shared" ref="R6:R16" si="5">$X$20*$X$19/$X$21 * ((I6-I$5)*10^2) / (LN(P6) - LN(Q6))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S6" s="43" t="e">
+        <v>605.04793819016447</v>
+      </c>
+      <c r="S6" s="43">
         <f>L6/N6</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T6" s="24" t="e">
+        <v>260.37183917558428</v>
+      </c>
+      <c r="T6" s="24">
         <f t="shared" ref="T6:T16" si="6">ABS(- $X$20*$X$19/$X$21 * ((I6 - I$5)*10^2) * (LN(P6) - LN(Q6))^-2 / Q6 )</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U6" t="e">
+        <v>273.61142830558993</v>
+      </c>
+      <c r="U6">
         <f>SQRT( (1/L$5 * S6)^2 + (L6/L$5^2 * S$5)^2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V6" s="38" t="e">
+        <v>8.5810310996589978E-2</v>
+      </c>
+      <c r="V6" s="38">
         <f>T6*U6</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W6" s="39" t="e">
+        <v>23.478681755123855</v>
+      </c>
+      <c r="W6" s="39">
         <f>R6/V6</f>
-        <v>#DIV/0!</v>
+        <v>25.770098359892895</v>
       </c>
     </row>
     <row r="7" spans="2:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -2329,53 +2337,53 @@
       <c r="I7">
         <v>3382.9299000000001</v>
       </c>
-      <c r="K7" s="32" t="e">
+      <c r="K7" s="32">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L7" s="44" t="e">
+        <v>4.1737213481420576E-7</v>
+      </c>
+      <c r="L7" s="44">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>3726.1424013250548</v>
       </c>
       <c r="M7" s="44">
         <f t="shared" si="2"/>
         <v>29659.558116780237</v>
       </c>
-      <c r="N7" s="45" t="e">
+      <c r="N7" s="45">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>16.409166148845959</v>
       </c>
       <c r="P7">
         <f>(F7*(2*G7+1)*E7*H7) / (F$5*(2*G$5+1)*E$5*H$5)</f>
         <v>4.7951439090679582</v>
       </c>
-      <c r="Q7" s="24" t="e">
+      <c r="Q7" s="24">
         <f>L7/$L$5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R7" s="36" t="e">
+        <v>0.56523635498745795</v>
+      </c>
+      <c r="R7" s="36">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S7" t="e">
+        <v>558.76506727236131</v>
+      </c>
+      <c r="S7">
         <f>L7/N7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T7" s="24" t="e">
+        <v>227.07688907075337</v>
+      </c>
+      <c r="T7" s="24">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U7" t="e">
+        <v>462.34705326214009</v>
+      </c>
+      <c r="U7">
         <f>SQRT( (1/L$5 * S7)^2 + (L7/L$5^2 * S$5)^2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V7" s="38" t="e">
+        <v>3.9315264284317107E-2</v>
+      </c>
+      <c r="V7" s="38">
         <f>T7*U7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W7" s="39" t="e">
+        <v>18.177296590076274</v>
+      </c>
+      <c r="W7" s="39">
         <f>R7/V7</f>
-        <v>#DIV/0!</v>
+        <v>30.739723286322668</v>
       </c>
     </row>
     <row r="8" spans="2:23" x14ac:dyDescent="0.4">
@@ -2402,53 +2410,53 @@
       <c r="I8">
         <v>3359.002</v>
       </c>
-      <c r="K8" s="32" t="e">
+      <c r="K8" s="32">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L8" s="44" t="e">
+        <v>1.3730028661423062E-7</v>
+      </c>
+      <c r="L8" s="44">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>1226.5198855398328</v>
       </c>
       <c r="M8" s="44">
         <f t="shared" si="2"/>
         <v>29677.80854811089</v>
       </c>
-      <c r="N8" s="45" t="e">
+      <c r="N8" s="45">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>5.5361910988165741</v>
       </c>
       <c r="P8">
         <f t="shared" ref="P8:P16" si="7">(F8*(2*G8+1)*E8*H8) / (F$5*(2*G$5+1)*E$5*H$5)</f>
         <v>1.4894660524107943</v>
       </c>
-      <c r="Q8" s="24" t="e">
+      <c r="Q8" s="24">
         <f t="shared" ref="Q8:Q16" si="8">L8/$L$5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R8" s="36" t="e">
+        <v>0.186056665245975</v>
+      </c>
+      <c r="R8" s="36">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S8" t="e">
+        <v>557.79288081214361</v>
+      </c>
+      <c r="S8">
         <f t="shared" ref="S8:S16" si="9">L8/N8</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T8" s="24" t="e">
+        <v>221.54579992768237</v>
+      </c>
+      <c r="T8" s="24">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U8" t="e">
+        <v>1441.2489018307504</v>
+      </c>
+      <c r="U8">
         <f t="shared" ref="U8:U16" si="10">SQRT( (1/L$5 * S8)^2 + (L8/L$5^2 * S$5)^2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V8" s="38" t="e">
+        <v>3.4181369528453964E-2</v>
+      </c>
+      <c r="V8" s="38">
         <f t="shared" ref="V8:V16" si="11">T8*U8</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W8" s="39" t="e">
+        <v>49.263861295955351</v>
+      </c>
+      <c r="W8" s="39">
         <f t="shared" ref="W8:W16" si="12">R8/V8</f>
-        <v>#DIV/0!</v>
+        <v>11.322557065942766</v>
       </c>
     </row>
     <row r="9" spans="2:23" x14ac:dyDescent="0.4">
@@ -2475,53 +2483,53 @@
       <c r="I9">
         <v>3287.2629000000002</v>
       </c>
-      <c r="K9" s="32" t="e">
+      <c r="K9" s="32">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L9" s="44" t="e">
+        <v>1.2815801252320444E-7</v>
+      </c>
+      <c r="L9" s="44">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>1146.7953169619516</v>
       </c>
       <c r="M9" s="44">
         <f t="shared" si="2"/>
         <v>29728.214501309831</v>
       </c>
-      <c r="N9" s="45" t="e">
+      <c r="N9" s="45">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>5.1778818651767047</v>
       </c>
       <c r="P9">
         <f t="shared" si="7"/>
         <v>1.1705616422925744</v>
       </c>
-      <c r="Q9" s="24" t="e">
+      <c r="Q9" s="24">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R9" s="36" t="e">
+        <v>0.17396286428713773</v>
+      </c>
+      <c r="R9" s="36">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S9" t="e">
+        <v>554.480760762459</v>
+      </c>
+      <c r="S9">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T9" s="24" t="e">
+        <v>221.47962174931064</v>
+      </c>
+      <c r="T9" s="24">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U9" t="e">
+        <v>1671.9241241640348</v>
+      </c>
+      <c r="U9">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V9" s="38" t="e">
+        <v>3.4099810599702421E-2</v>
+      </c>
+      <c r="V9" s="38">
         <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W9" s="39" t="e">
+        <v>57.012295971066941</v>
+      </c>
+      <c r="W9" s="39">
         <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
+        <v>9.725634642811988</v>
       </c>
     </row>
     <row r="10" spans="2:23" x14ac:dyDescent="0.4">
@@ -2548,53 +2556,53 @@
       <c r="I10">
         <v>3169.252</v>
       </c>
-      <c r="K10" s="32" t="e">
+      <c r="K10" s="32">
         <f>$F$27 * F10 * (2*G10+1) *$X$20*$X$19*(E10*10^2)*H10 * EXP(-((I10*10^2) * $X$20*$X$19)/($X$21*$F$20)) / (4*PI()*$X$23)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L10" s="44" t="e">
+        <v>1.6775212109651233E-7</v>
+      </c>
+      <c r="L10" s="44">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>1503.8595706475162</v>
       </c>
       <c r="M10" s="44">
         <f t="shared" si="2"/>
         <v>29782.965795301767</v>
       </c>
-      <c r="N10" s="45" t="e">
+      <c r="N10" s="45">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>6.7617344159958295</v>
       </c>
       <c r="P10">
         <f t="shared" si="7"/>
         <v>1.1545625272500089</v>
       </c>
-      <c r="Q10" s="24" t="e">
+      <c r="Q10" s="24">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R10" s="36" t="e">
+        <v>0.22812764799958365</v>
+      </c>
+      <c r="R10" s="36">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S10" t="e">
+        <v>547.16623520349742</v>
+      </c>
+      <c r="S10">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T10" s="24" t="e">
+        <v>222.40737037673733</v>
+      </c>
+      <c r="T10" s="24">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U10" t="e">
+        <v>1479.1263579353126</v>
+      </c>
+      <c r="U10">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V10" s="38" t="e">
+        <v>3.4594149115908988E-2</v>
+      </c>
+      <c r="V10" s="38">
         <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W10" s="39" t="e">
+        <v>51.169117787685579</v>
+      </c>
+      <c r="W10" s="39">
         <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
+        <v>10.693290384130467</v>
       </c>
     </row>
     <row r="11" spans="2:23" x14ac:dyDescent="0.4">
@@ -2623,53 +2631,53 @@
       <c r="I11">
         <v>3489.2150999999999</v>
       </c>
-      <c r="K11" s="32" t="e">
+      <c r="K11" s="32">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L11" s="44" t="e">
+        <v>1.3834490098855738E-7</v>
+      </c>
+      <c r="L11" s="44">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>1250.2551618634254</v>
       </c>
       <c r="M11" s="44">
         <f t="shared" si="2"/>
         <v>30023.697675234613</v>
       </c>
-      <c r="N11" s="45" t="e">
+      <c r="N11" s="45">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>5.6221962046988674</v>
       </c>
       <c r="P11">
         <f t="shared" si="7"/>
         <v>2.0508270783837399</v>
       </c>
-      <c r="Q11" s="24" t="e">
+      <c r="Q11" s="24">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R11" s="36" t="e">
+        <v>0.18965718278631291</v>
+      </c>
+      <c r="R11" s="36">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S11" t="e">
+        <v>566.04327713544274</v>
+      </c>
+      <c r="S11">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T11" s="24" t="e">
+        <v>222.37842941491417</v>
+      </c>
+      <c r="T11" s="24">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U11" t="e">
+        <v>1253.6058809047049</v>
+      </c>
+      <c r="U11">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V11" s="38" t="e">
+        <v>3.4327717491409664E-2</v>
+      </c>
+      <c r="V11" s="38">
         <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W11" s="39" t="e">
+        <v>43.033428525266459</v>
+      </c>
+      <c r="W11" s="39">
         <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
+        <v>13.153571456736211</v>
       </c>
     </row>
     <row r="12" spans="2:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -2696,53 +2704,53 @@
       <c r="I12">
         <v>3332.4121</v>
       </c>
-      <c r="K12" s="32" t="e">
+      <c r="K12" s="32">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L12" s="44" t="e">
+        <v>1.9681164983981956E-7</v>
+      </c>
+      <c r="L12" s="44">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>1778.6843026233107</v>
       </c>
       <c r="M12" s="44">
         <f t="shared" si="2"/>
         <v>30024.566743393221</v>
       </c>
-      <c r="N12" s="45" t="e">
+      <c r="N12" s="45">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>7.9559928756933136</v>
       </c>
       <c r="P12">
         <f t="shared" si="7"/>
         <v>2.0031739976454572</v>
       </c>
-      <c r="Q12" s="24" t="e">
+      <c r="Q12" s="24">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R12" s="36" t="e">
+        <v>0.26981712548900072</v>
+      </c>
+      <c r="R12" s="36">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S12" t="e">
+        <v>559.68256383508378</v>
+      </c>
+      <c r="S12">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T12" s="24" t="e">
+        <v>223.5653463262195</v>
+      </c>
+      <c r="T12" s="24">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U12" t="e">
+        <v>1034.6974779813047</v>
+      </c>
+      <c r="U12">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V12" s="38" t="e">
+        <v>3.5099483913847568E-2</v>
+      </c>
+      <c r="V12" s="38">
         <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W12" s="39" t="e">
+        <v>36.31734748410345</v>
+      </c>
+      <c r="W12" s="39">
         <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
+        <v>15.410887705388278</v>
       </c>
     </row>
     <row r="13" spans="2:23" x14ac:dyDescent="0.4">
@@ -2771,53 +2779,53 @@
       <c r="I13">
         <v>3196.0990999999999</v>
       </c>
-      <c r="K13" s="32" t="e">
+      <c r="K13" s="32">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L13" s="44" t="e">
+        <v>7.9711948995009023E-8</v>
+      </c>
+      <c r="L13" s="44">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>736.24389277806824</v>
       </c>
       <c r="M13" s="44">
         <f t="shared" si="2"/>
         <v>30685.058543930998</v>
       </c>
-      <c r="N13" s="45" t="e">
+      <c r="N13" s="45">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>3.3058488152838996</v>
       </c>
       <c r="P13">
         <f t="shared" si="7"/>
         <v>0.58510257915491859</v>
       </c>
-      <c r="Q13" s="24" t="e">
+      <c r="Q13" s="24">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R13" s="36" t="e">
+        <v>0.11168435596762598</v>
+      </c>
+      <c r="R13" s="36">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S13" t="e">
+        <v>559.0787060938444</v>
+      </c>
+      <c r="S13">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T13" s="24" t="e">
+        <v>222.70948670556223</v>
+      </c>
+      <c r="T13" s="24">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U13" t="e">
+        <v>3022.6738332367936</v>
+      </c>
+      <c r="U13">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V13" s="38" t="e">
+        <v>3.3990746346392722E-2</v>
+      </c>
+      <c r="V13" s="38">
         <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W13" s="39" t="e">
+        <v>102.74293955343043</v>
+      </c>
+      <c r="W13" s="39">
         <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
+        <v>5.4415292040880452</v>
       </c>
     </row>
     <row r="14" spans="2:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -2844,53 +2852,53 @@
       <c r="I14">
         <v>3081.1588999999999</v>
       </c>
-      <c r="K14" s="32" t="e">
+      <c r="K14" s="32">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L14" s="44" t="e">
+        <v>4.9701473280816603E-7</v>
+      </c>
+      <c r="L14" s="44">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>4594.2202127006813</v>
       </c>
       <c r="M14" s="44">
         <f t="shared" si="2"/>
         <v>30709.392452371849</v>
       </c>
-      <c r="N14" s="45" t="e">
+      <c r="N14" s="45">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>19.865920632916211</v>
       </c>
       <c r="P14">
         <f t="shared" si="7"/>
         <v>2.7693423850317664</v>
       </c>
-      <c r="Q14" s="24" t="e">
+      <c r="Q14" s="24">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R14" s="36" t="e">
+        <v>0.69691922834542785</v>
+      </c>
+      <c r="R14" s="36">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S14" t="e">
+        <v>551.22506762590479</v>
+      </c>
+      <c r="S14">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T14" s="24" t="e">
+        <v>231.26137960545523</v>
+      </c>
+      <c r="T14" s="24">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U14" t="e">
+        <v>573.27528473696339</v>
+      </c>
+      <c r="U14">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V14" s="38" t="e">
+        <v>4.2150346946034076E-2</v>
+      </c>
+      <c r="V14" s="38">
         <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W14" s="39" t="e">
+        <v>24.163752147249479</v>
+      </c>
+      <c r="W14" s="39">
         <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
+        <v>22.812064296423841</v>
       </c>
     </row>
     <row r="15" spans="2:23" x14ac:dyDescent="0.4">
@@ -2917,53 +2925,53 @@
       <c r="I15">
         <v>2999.355</v>
       </c>
-      <c r="K15" s="32" t="e">
+      <c r="K15" s="32">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L15" s="44" t="e">
+        <v>2.0287653363454703E-7</v>
+      </c>
+      <c r="L15" s="44">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>1877.8629854241192</v>
       </c>
       <c r="M15" s="44">
         <f t="shared" si="2"/>
         <v>30751.107723984769</v>
       </c>
-      <c r="N15" s="45" t="e">
+      <c r="N15" s="45">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>8.331080682007304</v>
       </c>
       <c r="P15">
         <f t="shared" si="7"/>
         <v>0.92906664077249623</v>
       </c>
-      <c r="Q15" s="24" t="e">
+      <c r="Q15" s="24">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R15" s="36" t="e">
+        <v>0.28486201404152917</v>
+      </c>
+      <c r="R15" s="36">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S15" t="e">
+        <v>543.76462868521344</v>
+      </c>
+      <c r="S15">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T15" s="24" t="e">
+        <v>225.40448917746693</v>
+      </c>
+      <c r="T15" s="24">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U15" t="e">
+        <v>1614.7096232520682</v>
+      </c>
+      <c r="U15">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V15" s="38" t="e">
+        <v>3.5501482539665549E-2</v>
+      </c>
+      <c r="V15" s="38">
         <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W15" s="39" t="e">
+        <v>57.324585496513237</v>
+      </c>
+      <c r="W15" s="39">
         <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
+        <v>9.4857140958880173</v>
       </c>
     </row>
     <row r="16" spans="2:23" x14ac:dyDescent="0.4">
@@ -2990,53 +2998,53 @@
       <c r="I16">
         <v>2928.3181</v>
       </c>
-      <c r="K16" s="32" t="e">
+      <c r="K16" s="32">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L16" s="44" t="e">
+        <v>1.2460391681109094E-7</v>
+      </c>
+      <c r="L16" s="44">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>1154.5630954495548</v>
       </c>
       <c r="M16" s="44">
         <f t="shared" si="2"/>
         <v>30783.263245853053</v>
       </c>
-      <c r="N16" s="45" t="e">
+      <c r="N16" s="45">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>5.1573820059390494</v>
       </c>
       <c r="P16">
         <f t="shared" si="7"/>
         <v>0.48124628561375116</v>
       </c>
-      <c r="Q16" s="24" t="e">
+      <c r="Q16" s="24">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R16" s="36" t="e">
+        <v>0.17514119574251139</v>
+      </c>
+      <c r="R16" s="36">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S16" t="e">
+        <v>534.84974768160976</v>
+      </c>
+      <c r="S16">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T16" s="24" t="e">
+        <v>223.86611930626873</v>
+      </c>
+      <c r="T16" s="24">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U16" t="e">
+        <v>3021.2312770497838</v>
+      </c>
+      <c r="U16">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V16" s="38" t="e">
+        <v>3.446325992321092E-2</v>
+      </c>
+      <c r="V16" s="38">
         <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W16" s="39" t="e">
+        <v>104.12147878910116</v>
+      </c>
+      <c r="W16" s="39">
         <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
+        <v>5.136785934100609</v>
       </c>
     </row>
     <row r="18" spans="2:24" x14ac:dyDescent="0.4">
@@ -3352,7 +3360,10 @@
       <c r="W23" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="X23" s="12"/>
+      <c r="X23" s="12">
+        <f>$U$26 * $F$20^0 + $U$27 * $F$20^1 + $U$28 * $F$20^2 + $U$29 * $F$20^3 + $U$30 * $F$20^4 + $U$31 * $F$20^5 + $U$32 * $F$20^6</f>
+        <v>106.38786872000001</v>
+      </c>
     </row>
     <row r="24" spans="2:24" x14ac:dyDescent="0.4">
       <c r="B24" s="7" t="s">
@@ -3433,9 +3444,10 @@
       <c r="R25" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="T25" t="s">
-        <v>80</v>
-      </c>
+      <c r="T25" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="U25" s="15"/>
       <c r="V25" s="39"/>
       <c r="W25"/>
     </row>
@@ -3479,6 +3491,12 @@
       </c>
       <c r="R26" s="9">
         <v>0.98</v>
+      </c>
+      <c r="T26" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="U26" s="22">
+        <v>-1.11391</v>
       </c>
       <c r="V26" s="39"/>
       <c r="W26"/>
@@ -3522,11 +3540,11 @@
       <c r="R27" s="9">
         <v>15</v>
       </c>
-      <c r="T27" t="s">
-        <v>192</v>
-      </c>
-      <c r="U27">
-        <v>7.36</v>
+      <c r="T27" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="U27" s="9">
+        <v>5.8107600000000002E-2</v>
       </c>
       <c r="V27" s="39"/>
       <c r="W27"/>
@@ -3559,11 +3577,11 @@
       <c r="R28" s="9">
         <v>0.5</v>
       </c>
-      <c r="T28" t="s">
-        <v>193</v>
-      </c>
-      <c r="U28">
-        <v>20.725999999999999</v>
+      <c r="T28" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="U28" s="9">
+        <v>3.0296700000000001E-4</v>
       </c>
       <c r="V28" s="39"/>
       <c r="W28"/>
@@ -3597,11 +3615,12 @@
         <f>$R$26^$R$27 * $R$28</f>
         <v>0.36928455132270177</v>
       </c>
-      <c r="T29" t="s">
-        <v>194</v>
-      </c>
-      <c r="U29">
-        <v>37.607999999999997</v>
+      <c r="T29" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="U29" s="9">
+        <f>-2.83724 *10^-7</f>
+        <v>-2.8372400000000001E-7</v>
       </c>
       <c r="V29" s="39"/>
       <c r="W29"/>
@@ -3621,11 +3640,12 @@
         <v>0.7</v>
       </c>
       <c r="M30" s="8"/>
-      <c r="T30" t="s">
-        <v>195</v>
-      </c>
-      <c r="U30">
-        <v>57.649000000000001</v>
+      <c r="T30" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="U30" s="9">
+        <f>+ 2.31119 * 10^-10</f>
+        <v>2.3111899999999999E-10</v>
       </c>
       <c r="V30" s="39"/>
       <c r="W30"/>
@@ -3659,11 +3679,12 @@
       <c r="R31" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="T31" t="s">
-        <v>196</v>
-      </c>
-      <c r="U31">
-        <v>80.578999999999994</v>
+      <c r="T31" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="U31" s="9">
+        <f>- 7.15895 * 10^-14</f>
+        <v>-7.1589500000000003E-14</v>
       </c>
       <c r="V31" s="39"/>
       <c r="W31"/>
@@ -3697,11 +3718,12 @@
       <c r="R32" s="22">
         <v>0.9</v>
       </c>
-      <c r="T32" t="s">
-        <v>197</v>
-      </c>
-      <c r="U32">
-        <v>106.393</v>
+      <c r="T32" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="U32" s="12">
+        <f xml:space="preserve"> + 1.0015 * 10^-17</f>
+        <v>1.0015000000000001E-17</v>
       </c>
       <c r="V32" s="39"/>
       <c r="W32"/>
@@ -3734,12 +3756,6 @@
       <c r="R33" s="12">
         <f>R21*R29*L32</f>
         <v>9.3952160689976222E-2</v>
-      </c>
-      <c r="T33" t="s">
-        <v>198</v>
-      </c>
-      <c r="U33">
-        <v>135.33000000000001</v>
       </c>
       <c r="V33" s="39"/>
       <c r="W33"/>
@@ -3851,12 +3867,9 @@
     <mergeCell ref="B11:B12"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
-  <dataValidations count="2">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F19" xr:uid="{C2605A09-1650-483D-820D-241861D95A0B}">
       <formula1>"T60, PLANETS"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F20" xr:uid="{0FCDD7A3-68B0-4DC3-A99D-3E7B638CFBD4}">
-      <formula1>"100, 200, 300, 400, 500, 600, 700, 800, 900, 1000, 1200"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>